<commit_message>
Read in and merged Cipriani dataset
</commit_message>
<xml_diff>
--- a/Full_Dataset_Cipriani_MA.xlsx
+++ b/Full_Dataset_Cipriani_MA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\OneDrive - University College London\Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents\apples_oranges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/rejucbu_ucl_ac_uk/Documents/Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents/apples_oranges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{75577818-B7A0-475A-9463-240E8DB4DC41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{570D4223-D9A5-44DF-9FA2-04B90C5540B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{CDC553A7-9840-4C64-A3B7-9DBCC61C43D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,9 +615,6 @@
     </r>
   </si>
   <si>
-    <t>change_N</t>
-  </si>
-  <si>
     <t>change_sd</t>
   </si>
   <si>
@@ -645,9 +642,6 @@
     <t>suicides</t>
   </si>
   <si>
-    <t>responders_no_missing</t>
-  </si>
-  <si>
     <t>change</t>
   </si>
   <si>
@@ -658,6 +652,12 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>responders_n_missing</t>
+  </si>
+  <si>
+    <t>change_n</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -958,35 +958,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1328,11 +1328,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="15.296875" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" customWidth="1"/>
@@ -1344,23 +1344,23 @@
     <col min="8" max="8" width="8.296875" customWidth="1"/>
     <col min="9" max="10" width="10.69921875" customWidth="1"/>
     <col min="11" max="11" width="9.296875" customWidth="1"/>
-    <col min="12" max="12" width="7.296875" customWidth="1"/>
-    <col min="13" max="13" width="7.59765625" customWidth="1"/>
+    <col min="12" max="12" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.19921875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.3984375" customWidth="1"/>
     <col min="15" max="15" width="10.8984375" customWidth="1"/>
     <col min="16" max="16" width="12.8984375" customWidth="1"/>
     <col min="17" max="17" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:17" ht="15" customHeight="1">
+      <c r="A1" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1368,44 +1368,44 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="60" t="s">
+      <c r="F1" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="61" t="s">
+      <c r="J1" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="K1" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="62" t="s">
+      <c r="O1" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="63" t="s">
+      <c r="Q1" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="64" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="12" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="16.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="12" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="16.5" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="12" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="16.5" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="14.25" customHeight="1">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="12" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>12</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="12" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="12" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="16.5" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="12" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="16.5" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="12" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="16.5" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="12" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>21</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="16.5" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="12" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>23</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="16.5" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="12" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>23</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="16.5" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="12" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="16.5" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="12" customHeight="1">
       <c r="A28" s="14" t="s">
         <v>23</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="16.5" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="12" customHeight="1">
       <c r="A30" s="14" t="s">
         <v>23</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="14.5" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>23</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="13.75" customHeight="1">
       <c r="A32" s="14" t="s">
         <v>23</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="16.5" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="12" customHeight="1">
       <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="16.5" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="14.25" customHeight="1">
       <c r="A36" s="33" t="s">
         <v>23</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="12" customHeight="1">
       <c r="A37" s="14" t="s">
         <v>23</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="16.5" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="12" customHeight="1">
       <c r="A39" s="14" t="s">
         <v>36</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="16.5" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="12" customHeight="1">
       <c r="A41" s="14" t="s">
         <v>37</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="16.5" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="12" customHeight="1">
       <c r="A43" s="14" t="s">
         <v>37</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="16.5" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>38</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="12" customHeight="1">
       <c r="A45" s="14" t="s">
         <v>38</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="16.5" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>39</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="12" customHeight="1">
       <c r="A47" s="14" t="s">
         <v>39</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="16.5" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>41</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="14.25" customHeight="1">
       <c r="A49" s="33" t="s">
         <v>41</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="12" customHeight="1">
       <c r="A50" s="14" t="s">
         <v>41</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="16.5" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>42</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="12" customHeight="1">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="16.5" customHeight="1">
       <c r="A53" s="3" t="s">
         <v>44</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="12" customHeight="1">
       <c r="A54" s="14" t="s">
         <v>44</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="16.5" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>45</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="12" customHeight="1">
       <c r="A56" s="14" t="s">
         <v>45</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="16.5" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>47</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="12" customHeight="1">
       <c r="A58" s="14" t="s">
         <v>47</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="16.5" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>48</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="12" customHeight="1">
       <c r="A60" s="14" t="s">
         <v>48</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="16.5" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>49</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="12" customHeight="1">
       <c r="A62" s="14" t="s">
         <v>49</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="16.5" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>50</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="12" customHeight="1">
       <c r="A64" s="14" t="s">
         <v>50</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="14.5" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>52</v>
       </c>
@@ -4807,10 +4807,10 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="15.296875" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" customWidth="1"/>
@@ -4822,23 +4822,23 @@
     <col min="8" max="8" width="8.296875" customWidth="1"/>
     <col min="9" max="10" width="10.69921875" customWidth="1"/>
     <col min="11" max="11" width="9.296875" customWidth="1"/>
-    <col min="12" max="12" width="7.09765625" customWidth="1"/>
-    <col min="13" max="13" width="7.796875" customWidth="1"/>
+    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.3984375" customWidth="1"/>
     <col min="15" max="15" width="10.8984375" customWidth="1"/>
     <col min="16" max="16" width="12.8984375" customWidth="1"/>
     <col min="17" max="17" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="12" customHeight="1">
       <c r="A1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="D1" s="13">
         <v>96</v>
@@ -4847,43 +4847,43 @@
         <v>10</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="20" t="s">
+      <c r="O1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="21" t="s">
+      <c r="Q1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>52</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="12" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>52</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="16.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="13" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>52</v>
       </c>
@@ -5087,24 +5087,24 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
+    <row r="6" spans="1:17" ht="26.5" customHeight="1">
+      <c r="A6" s="68"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5361,16 +5361,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7861D6-F925-474F-A05C-98D66B52AD1D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
+    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fair few changes Fixed merge in of Cipriani data Fixed spelling errors in our med dataset Removed data for TADS placebo condition under psy comparison row Inspected studies with missing COhens d after all the imputations, fixed offending studies
</commit_message>
<xml_diff>
--- a/Full_Dataset_Cipriani_MA.xlsx
+++ b/Full_Dataset_Cipriani_MA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/rejucbu_ucl_ac_uk/Documents/Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents/apples_oranges/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\OneDrive - University College London\Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents\apples_oranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{CDC553A7-9840-4C64-A3B7-9DBCC61C43D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{CDC553A7-9840-4C64-A3B7-9DBCC61C43D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{041D1B3D-68F9-41D0-8D97-C1CC6E641F00}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="88">
   <si>
     <r>
       <rPr>
@@ -658,6 +658,146 @@
   </si>
   <si>
     <t>change_n</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Wagner</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2003a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Placebo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5 (combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>179 (combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>95 (combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2003b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sertraline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>17 (combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>185 (combined)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Citalopram</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Escitalopram</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -667,7 +807,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -698,6 +838,21 @@
     <font>
       <sz val="6"/>
       <name val="Arial MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -780,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -986,6 +1141,213 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1326,13 +1688,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.296875" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" customWidth="1"/>
@@ -1352,7 +1714,7 @@
     <col min="17" max="17" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="66" t="s">
         <v>69</v>
       </c>
@@ -1405,7 +1767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5" customHeight="1">
+    <row r="2" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1458,7 +1820,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12" customHeight="1">
+    <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -1511,7 +1873,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5" customHeight="1">
+    <row r="4" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1564,7 +1926,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12" customHeight="1">
+    <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1979,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.5" customHeight="1">
+    <row r="6" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1670,7 +2032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12" customHeight="1">
+    <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -1723,7 +2085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5" customHeight="1">
+    <row r="8" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1776,7 +2138,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.25" customHeight="1">
+    <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -1829,7 +2191,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="12" customHeight="1">
+    <row r="10" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>12</v>
       </c>
@@ -1882,7 +2244,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1935,7 +2297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="12" customHeight="1">
+    <row r="12" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1988,7 +2350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16.5" customHeight="1">
+    <row r="13" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -2041,7 +2403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="12" customHeight="1">
+    <row r="14" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16.5" customHeight="1">
+    <row r="15" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -2147,7 +2509,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="12" customHeight="1">
+    <row r="16" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
@@ -2200,7 +2562,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16.5" customHeight="1">
+    <row r="17" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -2253,7 +2615,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="12" customHeight="1">
+    <row r="18" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2668,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16.5" customHeight="1">
+    <row r="19" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -2359,7 +2721,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="12" customHeight="1">
+    <row r="20" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>21</v>
       </c>
@@ -2412,7 +2774,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16.5" customHeight="1">
+    <row r="21" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -2465,7 +2827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="12" customHeight="1">
+    <row r="22" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>23</v>
       </c>
@@ -2518,7 +2880,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16.5" customHeight="1">
+    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -2571,7 +2933,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="12" customHeight="1">
+    <row r="24" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>23</v>
       </c>
@@ -2624,7 +2986,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16.5" customHeight="1">
+    <row r="25" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2677,7 +3039,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="12" customHeight="1">
+    <row r="26" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
@@ -2730,7 +3092,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16.5" customHeight="1">
+    <row r="27" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -2783,7 +3145,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="12" customHeight="1">
+    <row r="28" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>23</v>
       </c>
@@ -2836,7 +3198,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16.5" customHeight="1">
+    <row r="29" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -2889,7 +3251,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="12" customHeight="1">
+    <row r="30" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>23</v>
       </c>
@@ -2942,7 +3304,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="14.5" customHeight="1">
+    <row r="31" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>23</v>
       </c>
@@ -2995,7 +3357,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="13.75" customHeight="1">
+    <row r="32" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>23</v>
       </c>
@@ -3048,7 +3410,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="16.5" customHeight="1">
+    <row r="33" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
@@ -3101,7 +3463,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="12" customHeight="1">
+    <row r="34" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
@@ -3154,7 +3516,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="16.5" customHeight="1">
+    <row r="35" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
@@ -3207,7 +3569,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="14.25" customHeight="1">
+    <row r="36" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="33" t="s">
         <v>23</v>
       </c>
@@ -3260,7 +3622,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="12" customHeight="1">
+    <row r="37" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>23</v>
       </c>
@@ -3313,7 +3675,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="16.5" customHeight="1">
+    <row r="38" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -3366,7 +3728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="12" customHeight="1">
+    <row r="39" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>36</v>
       </c>
@@ -3419,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="16.5" customHeight="1">
+    <row r="40" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
@@ -3472,7 +3834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="12" customHeight="1">
+    <row r="41" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>37</v>
       </c>
@@ -3525,7 +3887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16.5" customHeight="1">
+    <row r="42" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
@@ -3578,7 +3940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="12" customHeight="1">
+    <row r="43" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>37</v>
       </c>
@@ -3631,7 +3993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16.5" customHeight="1">
+    <row r="44" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>38</v>
       </c>
@@ -3684,7 +4046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="12" customHeight="1">
+    <row r="45" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>38</v>
       </c>
@@ -3737,7 +4099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="16.5" customHeight="1">
+    <row r="46" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>39</v>
       </c>
@@ -3790,7 +4152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="12" customHeight="1">
+    <row r="47" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>39</v>
       </c>
@@ -3843,7 +4205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="16.5" customHeight="1">
+    <row r="48" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>41</v>
       </c>
@@ -3896,7 +4258,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="14.25" customHeight="1">
+    <row r="49" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>41</v>
       </c>
@@ -3949,7 +4311,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="12" customHeight="1">
+    <row r="50" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>41</v>
       </c>
@@ -4002,7 +4364,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16.5" customHeight="1">
+    <row r="51" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>42</v>
       </c>
@@ -4055,7 +4417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="12" customHeight="1">
+    <row r="52" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
@@ -4108,7 +4470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16.5" customHeight="1">
+    <row r="53" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>44</v>
       </c>
@@ -4161,7 +4523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="12" customHeight="1">
+    <row r="54" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>44</v>
       </c>
@@ -4214,7 +4576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="16.5" customHeight="1">
+    <row r="55" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>45</v>
       </c>
@@ -4267,7 +4629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="12" customHeight="1">
+    <row r="56" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
         <v>45</v>
       </c>
@@ -4320,7 +4682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="16.5" customHeight="1">
+    <row r="57" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>47</v>
       </c>
@@ -4373,7 +4735,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="12" customHeight="1">
+    <row r="58" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
         <v>47</v>
       </c>
@@ -4426,7 +4788,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="16.5" customHeight="1">
+    <row r="59" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>48</v>
       </c>
@@ -4479,7 +4841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="12" customHeight="1">
+    <row r="60" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="14" t="s">
         <v>48</v>
       </c>
@@ -4532,7 +4894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="16.5" customHeight="1">
+    <row r="61" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>49</v>
       </c>
@@ -4585,7 +4947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="12" customHeight="1">
+    <row r="62" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="14" t="s">
         <v>49</v>
       </c>
@@ -4638,7 +5000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="16.5" customHeight="1">
+    <row r="63" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>50</v>
       </c>
@@ -4691,7 +5053,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="12" customHeight="1">
+    <row r="64" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="14" t="s">
         <v>50</v>
       </c>
@@ -4744,7 +5106,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="14.5" customHeight="1">
+    <row r="65" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>52</v>
       </c>
@@ -4796,6 +5158,376 @@
       <c r="Q65" s="12">
         <v>97</v>
       </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A66" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="81">
+        <v>91</v>
+      </c>
+      <c r="E66" s="81">
+        <v>10</v>
+      </c>
+      <c r="F66" s="95">
+        <v>-22.1</v>
+      </c>
+      <c r="G66" s="83">
+        <v>14.71</v>
+      </c>
+      <c r="H66" s="84">
+        <v>88</v>
+      </c>
+      <c r="I66" s="91" t="s">
+        <v>77</v>
+      </c>
+      <c r="J66" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="K66" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="L66" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="M66" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="N66" s="87">
+        <v>14</v>
+      </c>
+      <c r="O66" s="87">
+        <v>91</v>
+      </c>
+      <c r="P66" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="88">
+        <v>91</v>
+      </c>
+      <c r="R66" s="70"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A67" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="73">
+        <v>92</v>
+      </c>
+      <c r="E67" s="73">
+        <v>10</v>
+      </c>
+      <c r="F67" s="93">
+        <v>-28.8</v>
+      </c>
+      <c r="G67" s="75">
+        <v>15.71</v>
+      </c>
+      <c r="H67" s="76">
+        <v>92</v>
+      </c>
+      <c r="I67" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="J67" s="89" t="s">
+        <v>85</v>
+      </c>
+      <c r="K67" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="L67" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="M67" s="101" t="s">
+        <v>81</v>
+      </c>
+      <c r="N67" s="79">
+        <v>14</v>
+      </c>
+      <c r="O67" s="79">
+        <v>92</v>
+      </c>
+      <c r="P67" s="94">
+        <v>2</v>
+      </c>
+      <c r="Q67" s="80">
+        <v>92</v>
+      </c>
+      <c r="R67" s="69"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A68" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="81">
+        <v>96</v>
+      </c>
+      <c r="E68" s="81">
+        <v>10</v>
+      </c>
+      <c r="F68" s="95">
+        <v>-25.6</v>
+      </c>
+      <c r="G68" s="83">
+        <v>15.71</v>
+      </c>
+      <c r="H68" s="84">
+        <v>91</v>
+      </c>
+      <c r="I68" s="91" t="s">
+        <v>77</v>
+      </c>
+      <c r="J68" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="K68" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="L68" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="M68" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="N68" s="87">
+        <v>17</v>
+      </c>
+      <c r="O68" s="87">
+        <v>96</v>
+      </c>
+      <c r="P68" s="96">
+        <v>2</v>
+      </c>
+      <c r="Q68" s="88">
+        <v>96</v>
+      </c>
+      <c r="R68" s="70"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A69" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="4">
+        <v>2004</v>
+      </c>
+      <c r="C69" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="73">
+        <v>93</v>
+      </c>
+      <c r="E69" s="73">
+        <v>8</v>
+      </c>
+      <c r="F69" s="93">
+        <v>-21.7</v>
+      </c>
+      <c r="G69" s="75">
+        <v>15.09</v>
+      </c>
+      <c r="H69" s="76">
+        <v>89</v>
+      </c>
+      <c r="I69" s="77">
+        <v>5</v>
+      </c>
+      <c r="J69" s="77">
+        <v>93</v>
+      </c>
+      <c r="K69" s="90">
+        <v>42</v>
+      </c>
+      <c r="L69" s="90">
+        <v>89</v>
+      </c>
+      <c r="M69" s="102"/>
+      <c r="N69" s="79">
+        <v>22</v>
+      </c>
+      <c r="O69" s="79">
+        <v>93</v>
+      </c>
+      <c r="P69" s="94">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="80">
+        <v>93</v>
+      </c>
+      <c r="R69" s="69"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A70" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="4">
+        <v>2004</v>
+      </c>
+      <c r="C70" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" s="81">
+        <v>85</v>
+      </c>
+      <c r="E70" s="81">
+        <v>8</v>
+      </c>
+      <c r="F70" s="95">
+        <v>-16.5</v>
+      </c>
+      <c r="G70" s="83">
+        <v>14.75</v>
+      </c>
+      <c r="H70" s="84">
+        <v>85</v>
+      </c>
+      <c r="I70" s="85">
+        <v>5</v>
+      </c>
+      <c r="J70" s="85">
+        <v>85</v>
+      </c>
+      <c r="K70" s="92">
+        <v>38</v>
+      </c>
+      <c r="L70" s="92">
+        <v>85</v>
+      </c>
+      <c r="M70" s="103"/>
+      <c r="N70" s="87">
+        <v>18</v>
+      </c>
+      <c r="O70" s="87">
+        <v>85</v>
+      </c>
+      <c r="P70" s="96">
+        <v>2</v>
+      </c>
+      <c r="Q70" s="88">
+        <v>85</v>
+      </c>
+      <c r="R70" s="70"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A71" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="4">
+        <v>2006</v>
+      </c>
+      <c r="C71" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="D71" s="73">
+        <v>132</v>
+      </c>
+      <c r="E71" s="73">
+        <v>8</v>
+      </c>
+      <c r="F71" s="93">
+        <v>-21.9</v>
+      </c>
+      <c r="G71" s="99">
+        <v>13.5</v>
+      </c>
+      <c r="H71" s="76">
+        <v>129</v>
+      </c>
+      <c r="I71" s="77">
+        <v>2</v>
+      </c>
+      <c r="J71" s="77">
+        <v>132</v>
+      </c>
+      <c r="K71" s="90">
+        <v>81</v>
+      </c>
+      <c r="L71" s="90">
+        <v>129</v>
+      </c>
+      <c r="M71" s="102"/>
+      <c r="N71" s="79">
+        <v>30</v>
+      </c>
+      <c r="O71" s="79">
+        <v>132</v>
+      </c>
+      <c r="P71" s="94">
+        <v>1</v>
+      </c>
+      <c r="Q71" s="80">
+        <v>132</v>
+      </c>
+      <c r="R71" s="69"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A72" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="4">
+        <v>2006</v>
+      </c>
+      <c r="C72" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" s="81">
+        <v>136</v>
+      </c>
+      <c r="E72" s="81">
+        <v>8</v>
+      </c>
+      <c r="F72" s="95">
+        <v>-20.2</v>
+      </c>
+      <c r="G72" s="97">
+        <v>13.5</v>
+      </c>
+      <c r="H72" s="84">
+        <v>132</v>
+      </c>
+      <c r="I72" s="85">
+        <v>2</v>
+      </c>
+      <c r="J72" s="85">
+        <v>136</v>
+      </c>
+      <c r="K72" s="92">
+        <v>69</v>
+      </c>
+      <c r="L72" s="92">
+        <v>132</v>
+      </c>
+      <c r="M72" s="104"/>
+      <c r="N72" s="87">
+        <v>21</v>
+      </c>
+      <c r="O72" s="87">
+        <v>136</v>
+      </c>
+      <c r="P72" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="88">
+        <v>136</v>
+      </c>
+      <c r="R72" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4804,13 +5536,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.296875" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" customWidth="1"/>
@@ -4830,7 +5562,7 @@
     <col min="17" max="17" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12" customHeight="1">
+    <row r="1" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>69</v>
       </c>
@@ -4883,7 +5615,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5" customHeight="1">
+    <row r="2" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>52</v>
       </c>
@@ -4934,7 +5666,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12" customHeight="1">
+    <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>52</v>
       </c>
@@ -4985,7 +5717,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.25" customHeight="1">
+    <row r="4" spans="1:17" ht="16.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -5036,7 +5768,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="13" customHeight="1">
+    <row r="5" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>52</v>
       </c>
@@ -5087,7 +5819,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="26.5" customHeight="1">
+    <row r="6" spans="1:17" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -5106,6 +5838,376 @@
       <c r="P6" s="68"/>
       <c r="Q6" s="68"/>
     </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A66" s="115" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="114">
+        <v>91</v>
+      </c>
+      <c r="E66" s="114">
+        <v>10</v>
+      </c>
+      <c r="F66" s="128">
+        <v>-22.1</v>
+      </c>
+      <c r="G66" s="116">
+        <v>14.71</v>
+      </c>
+      <c r="H66" s="117">
+        <v>88</v>
+      </c>
+      <c r="I66" s="124" t="s">
+        <v>77</v>
+      </c>
+      <c r="J66" s="124" t="s">
+        <v>78</v>
+      </c>
+      <c r="K66" s="119" t="s">
+        <v>79</v>
+      </c>
+      <c r="L66" s="119" t="s">
+        <v>80</v>
+      </c>
+      <c r="M66" s="133" t="s">
+        <v>81</v>
+      </c>
+      <c r="N66" s="120">
+        <v>14</v>
+      </c>
+      <c r="O66" s="120">
+        <v>91</v>
+      </c>
+      <c r="P66" s="129">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="121">
+        <v>91</v>
+      </c>
+      <c r="R66" s="72"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A67" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="105" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="107" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="106">
+        <v>92</v>
+      </c>
+      <c r="E67" s="106">
+        <v>10</v>
+      </c>
+      <c r="F67" s="126">
+        <v>-28.8</v>
+      </c>
+      <c r="G67" s="108">
+        <v>15.71</v>
+      </c>
+      <c r="H67" s="109">
+        <v>92</v>
+      </c>
+      <c r="I67" s="122" t="s">
+        <v>84</v>
+      </c>
+      <c r="J67" s="122" t="s">
+        <v>85</v>
+      </c>
+      <c r="K67" s="111" t="s">
+        <v>84</v>
+      </c>
+      <c r="L67" s="111" t="s">
+        <v>80</v>
+      </c>
+      <c r="M67" s="134" t="s">
+        <v>81</v>
+      </c>
+      <c r="N67" s="112">
+        <v>14</v>
+      </c>
+      <c r="O67" s="112">
+        <v>92</v>
+      </c>
+      <c r="P67" s="127">
+        <v>2</v>
+      </c>
+      <c r="Q67" s="113">
+        <v>92</v>
+      </c>
+      <c r="R67" s="71"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A68" s="115" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="105" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="114">
+        <v>96</v>
+      </c>
+      <c r="E68" s="114">
+        <v>10</v>
+      </c>
+      <c r="F68" s="128">
+        <v>-25.6</v>
+      </c>
+      <c r="G68" s="116">
+        <v>15.71</v>
+      </c>
+      <c r="H68" s="117">
+        <v>91</v>
+      </c>
+      <c r="I68" s="124" t="s">
+        <v>77</v>
+      </c>
+      <c r="J68" s="124" t="s">
+        <v>78</v>
+      </c>
+      <c r="K68" s="119" t="s">
+        <v>79</v>
+      </c>
+      <c r="L68" s="119" t="s">
+        <v>80</v>
+      </c>
+      <c r="M68" s="133" t="s">
+        <v>81</v>
+      </c>
+      <c r="N68" s="120">
+        <v>17</v>
+      </c>
+      <c r="O68" s="120">
+        <v>96</v>
+      </c>
+      <c r="P68" s="129">
+        <v>2</v>
+      </c>
+      <c r="Q68" s="121">
+        <v>96</v>
+      </c>
+      <c r="R68" s="72"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A69" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="105">
+        <v>2004</v>
+      </c>
+      <c r="C69" s="131" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="106">
+        <v>93</v>
+      </c>
+      <c r="E69" s="106">
+        <v>8</v>
+      </c>
+      <c r="F69" s="126">
+        <v>-21.7</v>
+      </c>
+      <c r="G69" s="108">
+        <v>15.09</v>
+      </c>
+      <c r="H69" s="109">
+        <v>89</v>
+      </c>
+      <c r="I69" s="110">
+        <v>5</v>
+      </c>
+      <c r="J69" s="110">
+        <v>93</v>
+      </c>
+      <c r="K69" s="123">
+        <v>42</v>
+      </c>
+      <c r="L69" s="123">
+        <v>89</v>
+      </c>
+      <c r="M69" s="135"/>
+      <c r="N69" s="112">
+        <v>22</v>
+      </c>
+      <c r="O69" s="112">
+        <v>93</v>
+      </c>
+      <c r="P69" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="113">
+        <v>93</v>
+      </c>
+      <c r="R69" s="71"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A70" s="115" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="105">
+        <v>2004</v>
+      </c>
+      <c r="C70" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" s="114">
+        <v>85</v>
+      </c>
+      <c r="E70" s="114">
+        <v>8</v>
+      </c>
+      <c r="F70" s="128">
+        <v>-16.5</v>
+      </c>
+      <c r="G70" s="116">
+        <v>14.75</v>
+      </c>
+      <c r="H70" s="117">
+        <v>85</v>
+      </c>
+      <c r="I70" s="118">
+        <v>5</v>
+      </c>
+      <c r="J70" s="118">
+        <v>85</v>
+      </c>
+      <c r="K70" s="125">
+        <v>38</v>
+      </c>
+      <c r="L70" s="125">
+        <v>85</v>
+      </c>
+      <c r="M70" s="136"/>
+      <c r="N70" s="120">
+        <v>18</v>
+      </c>
+      <c r="O70" s="120">
+        <v>85</v>
+      </c>
+      <c r="P70" s="129">
+        <v>2</v>
+      </c>
+      <c r="Q70" s="121">
+        <v>85</v>
+      </c>
+      <c r="R70" s="72"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A71" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="105">
+        <v>2006</v>
+      </c>
+      <c r="C71" s="131" t="s">
+        <v>87</v>
+      </c>
+      <c r="D71" s="106">
+        <v>132</v>
+      </c>
+      <c r="E71" s="106">
+        <v>8</v>
+      </c>
+      <c r="F71" s="126">
+        <v>-21.9</v>
+      </c>
+      <c r="G71" s="132">
+        <v>13.5</v>
+      </c>
+      <c r="H71" s="109">
+        <v>129</v>
+      </c>
+      <c r="I71" s="110">
+        <v>2</v>
+      </c>
+      <c r="J71" s="110">
+        <v>132</v>
+      </c>
+      <c r="K71" s="123">
+        <v>81</v>
+      </c>
+      <c r="L71" s="123">
+        <v>129</v>
+      </c>
+      <c r="M71" s="135"/>
+      <c r="N71" s="112">
+        <v>30</v>
+      </c>
+      <c r="O71" s="112">
+        <v>132</v>
+      </c>
+      <c r="P71" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q71" s="113">
+        <v>132</v>
+      </c>
+      <c r="R71" s="71"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A72" s="115" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="105">
+        <v>2006</v>
+      </c>
+      <c r="C72" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" s="114">
+        <v>136</v>
+      </c>
+      <c r="E72" s="114">
+        <v>8</v>
+      </c>
+      <c r="F72" s="128">
+        <v>-20.2</v>
+      </c>
+      <c r="G72" s="130">
+        <v>13.5</v>
+      </c>
+      <c r="H72" s="117">
+        <v>132</v>
+      </c>
+      <c r="I72" s="118">
+        <v>2</v>
+      </c>
+      <c r="J72" s="118">
+        <v>136</v>
+      </c>
+      <c r="K72" s="125">
+        <v>69</v>
+      </c>
+      <c r="L72" s="125">
+        <v>132</v>
+      </c>
+      <c r="M72" s="137"/>
+      <c r="N72" s="120">
+        <v>21</v>
+      </c>
+      <c r="O72" s="120">
+        <v>136</v>
+      </c>
+      <c r="P72" s="129">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="121">
+        <v>136</v>
+      </c>
+      <c r="R72" s="72"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A6:Q6"/>
@@ -5115,23 +6217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE7BC97E19D5434CB0B01A1ABCBF2DDD" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e75b4284d528a6b18ce77feafc1e78ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xmlns:ns4="e7bbc584-5a77-4c67-8fd7-7058eeaacc07" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d1a975e0f863fb9b7e4676b30af5bf6" ns3:_="" ns4:_="">
     <xsd:import namespace="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
@@ -5358,32 +6443,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7861D6-F925-474F-A05C-98D66B52AD1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
-    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E94A216-E890-4AD8-8C39-4A01739F14DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E06423B4-F76C-45BC-8FC0-F8FBBD5863C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5400,4 +6477,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E94A216-E890-4AD8-8C39-4A01739F14DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7861D6-F925-474F-A05C-98D66B52AD1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
+    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>